<commit_message>
Updating 3 additional variables, sent by Chris on 5/5/2020
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15405" windowHeight="6630"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15405" windowHeight="6630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="DRC-BDRC" sheetId="5" r:id="rId2"/>
     <sheet name="DRC-PADRC" sheetId="2" r:id="rId3"/>
-    <sheet name="CPUC IRP" sheetId="11" r:id="rId4"/>
+    <sheet name="CPUC IRP for BAU" sheetId="11" r:id="rId4"/>
     <sheet name="Potential calculations" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Source:</t>
   </si>
@@ -56,27 +56,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>http://www.cpuc.ca.gov/uploadedFiles/CPUCWebsite/Content/UtilitiesIndustries/Energy/EnergyPrograms/ElectPowerProcurementGeneration/DemandModeling/IRP_RSP_2017IEPR_SERVM_results_20180913.pdf</t>
-  </si>
-  <si>
-    <t>IRP Production Cost Modeling with the Reference System Plan and the 2017 IPER: SERVM model results</t>
-  </si>
-  <si>
-    <t>2018 (Sept 18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The CPUC modeling to get to the 60% RPS / ~42 MMT (not counting CHP) level indicates </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a 2030 level of </t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>See "CPUC IRP" tab for details.</t>
-  </si>
-  <si>
     <t>Integrated Resource Plan and Long Term Procurement Planning Process (IRP Process)</t>
   </si>
   <si>
@@ -89,12 +68,6 @@
     <t>avg</t>
   </si>
   <si>
-    <t>Background on potential additional</t>
-  </si>
-  <si>
-    <t>Main Source</t>
-  </si>
-  <si>
     <t>Additional potential is specified based on Figure 41 of the LBNL report (shown below).</t>
   </si>
   <si>
@@ -135,13 +108,46 @@
   </si>
   <si>
     <t>In MW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From slide 85 of this presentation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We designate demand response to be the peak load shifting variety which may contribute to system flexibility. </t>
+  </si>
+  <si>
+    <t>The BAU Scenario does not envision the availability of such demand response - shift resources being added.</t>
+  </si>
+  <si>
+    <t>This is evident in the exceprt below from the CPUC's long run planning work, which shows all resources added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to provide flexiblity (to provide resource adequacy, in the CPUC terminology). </t>
+  </si>
+  <si>
+    <t>https://www.cpuc.ca.gov/uploadedFiles/CPUCWebsite/Content/UtilitiesIndustries/Energy/EnergyPrograms/ElectPowerProcurementGeneration/irp/2018/2019%20IRP%20Proposed%20Reference%20System%20Plan_20191106.pdf</t>
+  </si>
+  <si>
+    <t>2019-20 IRP: Proposed Reference System Plan</t>
+  </si>
+  <si>
+    <t>BAU capacity</t>
+  </si>
+  <si>
+    <t>Potential capacity</t>
+  </si>
+  <si>
+    <t>Slide 85</t>
+  </si>
+  <si>
+    <t>Amount of demand response shift added through 2030 implied:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +167,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -202,11 +224,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -299,11 +328,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="263986176"/>
-        <c:axId val="263996160"/>
+        <c:axId val="308521216"/>
+        <c:axId val="308547584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="263986176"/>
+        <c:axId val="308521216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,12 +342,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263996160"/>
+        <c:crossAx val="308547584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263996160"/>
+        <c:axId val="308547584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -329,7 +358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263986176"/>
+        <c:crossAx val="308521216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -353,40 +382,57 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>118050</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 1" descr="cid:image001.png@01D6223B.E3EE7A00"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="368300"/>
-          <a:ext cx="6775450" cy="4905950"/>
+          <a:off x="0" y="1085850"/>
+          <a:ext cx="5972175" cy="4443413"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -792,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -818,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
@@ -827,83 +873,68 @@
       </c>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B6" s="10">
+        <v>43775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="6"/>
+      <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>1753</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId1" display="https://www.cpuc.ca.gov/uploadedFiles/CPUCWebsite/Content/UtilitiesIndustries/Energy/EnergyPrograms/ElectPowerProcurementGeneration/irp/2018/2019 IRP Proposed Reference System Plan_20191106.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -917,9 +948,7 @@
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1044,148 +1073,148 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="C2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="E2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="F2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="G2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="H2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="I2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="J2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="K2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="L2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="M2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="N2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="O2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="P2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="R2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="S2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="T2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="U2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="V2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="W2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="X2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <f>'CPUC IRP'!$Q$13</f>
-        <v>1753</v>
+        <f>'CPUC IRP for BAU'!$G$6</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1201,7 +1230,7 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1473,42 +1502,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="O11:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="O12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12">
         <v>1752</v>
       </c>
     </row>
-    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="O13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q13">
         <v>1754</v>
       </c>
     </row>
-    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="P13" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q13">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="P14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14">
         <f>1753</f>
         <v>1753</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" display="https://www.cpuc.ca.gov/uploadedFiles/CPUCWebsite/Content/UtilitiesIndustries/Energy/EnergyPrograms/ElectPowerProcurementGeneration/irp/2018/2019 IRP Proposed Reference System Plan_20191106.pdf"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1516,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1580,7 +1654,7 @@
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1637,7 +1711,7 @@
     </row>
     <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <f>E2*1000</f>
@@ -1686,32 +1760,32 @@
     </row>
     <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
@@ -1724,7 +1798,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>0.5</v>
@@ -1735,12 +1809,12 @@
     </row>
     <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1796,7 +1870,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <f>0.513*B21</f>
@@ -1851,7 +1925,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <f>0.2994*B23</f>
@@ -1906,7 +1980,7 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>